<commit_message>
changed backlog and burn down
</commit_message>
<xml_diff>
--- a/ProductBurndown.xlsx
+++ b/ProductBurndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\AEC\AECProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60A03E3-350A-420D-A56D-513F88443320}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A96DF5B-3D62-4C6C-9A13-3A5DCFA90CA5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Initial</t>
   </si>
@@ -85,82 +85,6 @@
   <si>
     <t>Velocity (stpts / hour)</t>
   </si>
-  <si>
-    <t>Story ID</t>
-  </si>
-  <si>
-    <t>Story</t>
-  </si>
-  <si>
-    <t>Storypoints</t>
-  </si>
-  <si>
-    <t>Wechseln auf neues DevKit</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>Verbesserung tracking impl. (Canvas)</t>
-  </si>
-  <si>
-    <t>Implementation von Collision Detection</t>
-  </si>
-  <si>
-    <t>Tracking und Animation in 1 Projekt</t>
-  </si>
-  <si>
-    <t>Starten von Animation durch stehen auf homebutton</t>
-  </si>
-  <si>
-    <t>Auswahl von Text durch User</t>
-  </si>
-  <si>
-    <t>Animation Text auf smartphone</t>
-  </si>
-  <si>
-    <t>Smartphone fade out End of scene 1</t>
-  </si>
-  <si>
-    <t>Text converten mit rotX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animation for encryption
-</t>
-  </si>
-  <si>
-    <t>Selection of rotX with tracking End of scene 2</t>
-  </si>
-  <si>
-    <t>Implement Game scene 3</t>
-  </si>
-  <si>
-    <t>Create Animation of sending a message scene 4</t>
-  </si>
-  <si>
-    <t>Create Animation message tower</t>
-  </si>
-  <si>
-    <t>Leaderboard scene 5</t>
-  </si>
-  <si>
-    <t>Making Storys and Pm sheet</t>
-  </si>
-  <si>
-    <t>Done if animation 1 start when a user stands on the Home button of the Smartphone</t>
-  </si>
-  <si>
-    <t>Done if User can chose one of four text Bubbles and encrypt it</t>
-  </si>
-  <si>
-    <t>Done if a Text can get convertet fia rotX</t>
-  </si>
-  <si>
-    <t>Done if the model and the animation of the enryption work</t>
-  </si>
-  <si>
-    <t>Done when the User can choose a letter for the encryption</t>
-  </si>
 </sst>
 </file>
 
@@ -171,7 +95,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,33 +106,21 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,14 +133,8 @@
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -251,34 +157,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -286,7 +164,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -322,49 +200,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -439,96 +274,96 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Tabelle1!$A$7:$A$25</c:f>
+              <c:f>Tabelle1!$A$7:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>mmm\ d", "yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
+                  <c:v>43857</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>43871</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>43885</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>43899</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="m/d/yyyy">
+                <c:pt idx="4">
                   <c:v>43913</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>43927</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>43941</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>43955</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>43969</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>43983</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="m/d/yyyy">
+                <c:pt idx="10">
                   <c:v>43997</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="m/d/yyyy">
+                <c:pt idx="11">
                   <c:v>44011</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>44025</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>44039</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="m/d/yyyy">
+                <c:pt idx="14">
                   <c:v>44053</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="m/d/yyyy">
+                <c:pt idx="15">
                   <c:v>44067</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>44081</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="m/d/yyyy">
+                <c:pt idx="17">
                   <c:v>44095</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>44109</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44123</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$J$7:$J$25</c:f>
+              <c:f>Tabelle1!$J$7:$J$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
+                <c:ptCount val="46"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.1428571428571432</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>14.142857142857142</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>7.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.42857142857142883</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -571,7 +406,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1B87-4D66-B578-A6098CB7A188}"/>
+              <c16:uniqueId val="{00000000-BFAC-4661-BA3E-5976BEC8BA1C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -713,8 +548,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>371160</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>132551</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>84060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -753,8 +588,14 @@
       <sheetName val="Sheet 1 - Drawings"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="J2" t="str">
+            <v>Open Story Points at End</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
@@ -1082,28 +923,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="33.42578125" customWidth="1"/>
-    <col min="28" max="28" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:28" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1117,7 +956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>39</v>
       </c>
@@ -1132,22 +971,22 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-    </row>
-    <row r="6" spans="1:28" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+    </row>
+    <row r="6" spans="1:11" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1181,32 +1020,17 @@
       <c r="K6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="X6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-    </row>
-    <row r="7" spans="1:28" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>43871</v>
+        <v>43857</v>
       </c>
       <c r="B7" s="6">
         <v>30</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="6">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6">
-        <v>30</v>
-      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
       <c r="F7" s="7">
         <f>A3</f>
         <v>39</v>
@@ -1216,200 +1040,156 @@
       </c>
       <c r="H7" s="7">
         <f t="shared" ref="H7:H25" si="0">G7+D7</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I7" s="7">
         <f>'[1]Sheet 1 - Initial'!C7</f>
         <v>0</v>
       </c>
-      <c r="J7" s="7">
-        <f>MAX(IF(OR(ISBLANK(D7),ISBLANK(E7)),F7-K6*B7,F7-D7),0)</f>
-        <v>29</v>
+      <c r="J7" s="8">
+        <f>A3</f>
+        <v>39</v>
       </c>
       <c r="K7" s="9">
         <f>IF(OR(ISBLANK(D7),ISBLANK(E7)),'[1]Sheet 1 - Initial'!D7,H7/(I7+E7))</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="W7" s="15">
-        <v>1</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y7" s="16">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <f>A7+14</f>
-        <v>43885</v>
+        <v>43871</v>
       </c>
       <c r="B8" s="6">
         <v>30</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="6">
+        <v>10</v>
+      </c>
+      <c r="E8" s="6">
+        <v>30</v>
+      </c>
       <c r="F8" s="8">
         <f>J7+C8</f>
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="G8" s="7">
         <f>H7</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H8" s="7">
-        <f t="shared" si="0"/>
+        <f>G8+D8</f>
         <v>10</v>
       </c>
       <c r="I8" s="7">
         <f t="shared" ref="I8:I25" si="1">I7+E7</f>
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="J8" s="7">
         <f>MAX(IF(OR(ISBLANK(D8),ISBLANK(E8)),F8-K7*B8,F8-D8),0)</f>
+        <v>29</v>
+      </c>
+      <c r="K8" s="9">
+        <f>IF(OR(ISBLANK(D8),ISBLANK(E8)),K7,H8/(I8+E8))</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f t="shared" ref="A9:A25" si="2">A8+14</f>
+        <v>43885</v>
+      </c>
+      <c r="B9" s="6">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7">
+        <f t="shared" ref="F9:F25" si="3">J8+C9</f>
+        <v>29</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" ref="G9:G52" si="4">H8</f>
+        <v>10</v>
+      </c>
+      <c r="H9" s="7">
+        <f>G9+D9</f>
+        <v>10</v>
+      </c>
+      <c r="I9" s="7">
+        <f>I8+E8</f>
+        <v>30</v>
+      </c>
+      <c r="J9" s="7">
+        <f>MAX(IF(OR(ISBLANK(D9),ISBLANK(E9)),F9-K8*B9,F9-D9),0)</f>
         <v>19</v>
       </c>
-      <c r="K8" s="9">
-        <f t="shared" ref="K8:K25" si="2">IF(OR(ISBLANK(D8),ISBLANK(E8)),K7,H8/(I8+E8))</f>
+      <c r="K9" s="9">
+        <f>IF(OR(ISBLANK(D9),ISBLANK(E9)),K8,H9/(I9+E9))</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W8" s="15">
-        <v>2</v>
-      </c>
-      <c r="X8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y8" s="16">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <f t="shared" ref="A9:A25" si="3">A8+14</f>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" si="2"/>
         <v>43899</v>
       </c>
-      <c r="B9" s="6">
-        <v>30</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6">
+      <c r="B10" s="6">
+        <v>30</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
         <v>6</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E10" s="6">
         <v>40</v>
       </c>
-      <c r="F9" s="7">
-        <f t="shared" ref="F9:F25" si="4">J8+C9</f>
+      <c r="F10" s="7">
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="G9" s="7">
-        <f t="shared" ref="G9:G25" si="5">H8</f>
+      <c r="G10" s="7">
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="H9" s="7">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="I9" s="7">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="J9" s="7">
-        <f t="shared" ref="J9:J25" si="6">MAX(IF(OR(ISBLANK(D9),ISBLANK(E9)),F9-K8*B9,F9-D9),0)</f>
+      <c r="H10" s="7">
+        <f>G10+D10</f>
+        <v>16</v>
+      </c>
+      <c r="I10" s="7">
+        <f>I9+E9</f>
+        <v>30</v>
+      </c>
+      <c r="J10" s="7">
+        <f>MAX(IF(OR(ISBLANK(D10),ISBLANK(E10)),F10-K9*B10,F10-D10),0)</f>
         <v>13</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K10" s="9">
+        <f>IF(OR(ISBLANK(D10),ISBLANK(E10)),K9,H10/(I10+E10))</f>
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W9" s="15">
-        <v>3</v>
-      </c>
-      <c r="X9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y9" s="16">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-    </row>
-    <row r="10" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="27">
-        <f>A9+14</f>
         <v>43913</v>
       </c>
-      <c r="B10" s="6">
-        <v>30</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="7">
-        <f t="shared" si="4"/>
-        <v>13</v>
-      </c>
-      <c r="G10" s="7">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="H10" s="7">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="I10" s="7">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="J10" s="7">
-        <f t="shared" si="6"/>
-        <v>6.1428571428571432</v>
-      </c>
-      <c r="K10" s="9">
-        <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W10" s="15">
-        <v>4</v>
-      </c>
-      <c r="X10" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y10" s="16">
-        <v>2</v>
-      </c>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <f t="shared" si="3"/>
-        <v>43927</v>
-      </c>
       <c r="B11" s="6">
         <v>30</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <v>8</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="7">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="4"/>
-        <v>6.1428571428571432</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H11" s="7">
@@ -1417,36 +1197,22 @@
         <v>16</v>
       </c>
       <c r="I11" s="7">
-        <f t="shared" si="1"/>
+        <f>I10+E10</f>
         <v>70</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="J11:J25" si="5">MAX(IF(OR(ISBLANK(D11),ISBLANK(E11)),F11-K10*B11,F11-D11),0)</f>
+        <v>14.142857142857142</v>
       </c>
       <c r="K11" s="9">
+        <f t="shared" ref="K11:K25" si="6">IF(OR(ISBLANK(D11),ISBLANK(E11)),K10,H11/(I11+E11))</f>
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W11" s="15">
-        <v>5</v>
-      </c>
-      <c r="X11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y11" s="16">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <f t="shared" si="3"/>
-        <v>43941</v>
+        <v>43927</v>
       </c>
       <c r="B12" s="6">
         <v>30</v>
@@ -1455,11 +1221,11 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="7">
+        <f t="shared" si="3"/>
+        <v>14.142857142857142</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H12" s="7">
@@ -1471,32 +1237,18 @@
         <v>70</v>
       </c>
       <c r="J12" s="7">
+        <f t="shared" si="5"/>
+        <v>7.2857142857142856</v>
+      </c>
+      <c r="K12" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W12" s="15">
-        <v>6</v>
-      </c>
-      <c r="X12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y12" s="16">
-        <v>2</v>
-      </c>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <f t="shared" si="3"/>
-        <v>43955</v>
+        <v>43941</v>
       </c>
       <c r="B13" s="6">
         <v>30</v>
@@ -1505,11 +1257,11 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>7.2857142857142856</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H13" s="7">
@@ -1521,29 +1273,18 @@
         <v>70</v>
       </c>
       <c r="J13" s="7">
-        <f>MAX(IF(OR(ISBLANK(D13),ISBLANK(E13)),F13-K12*B13,F13-D13),0)</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.42857142857142883</v>
       </c>
       <c r="K13" s="9">
+        <f t="shared" si="6"/>
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W13" s="15">
-        <v>7</v>
-      </c>
-      <c r="X13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y13" s="16">
-        <v>2</v>
-      </c>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-    </row>
-    <row r="14" spans="1:28" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <f t="shared" si="3"/>
-        <v>43969</v>
+        <v>43955</v>
       </c>
       <c r="B14" s="6">
         <v>30</v>
@@ -1552,11 +1293,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7">
-        <f>J13+C14</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>0.42857142857142883</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="H14" s="7">
@@ -1568,31 +1309,18 @@
         <v>70</v>
       </c>
       <c r="J14" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K14" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W14" s="15">
-        <v>8</v>
-      </c>
-      <c r="X14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y14" s="16">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <f t="shared" si="3"/>
-        <v>43983</v>
+        <v>43969</v>
       </c>
       <c r="B15" s="6">
         <v>30</v>
@@ -1601,11 +1329,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H15" s="7">
@@ -1617,34 +1345,18 @@
         <v>70</v>
       </c>
       <c r="J15" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W15" s="15">
-        <v>9</v>
-      </c>
-      <c r="X15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y15" s="16">
-        <v>2</v>
-      </c>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27">
-        <f>A15+14</f>
-        <v>43997</v>
+        <v>43983</v>
       </c>
       <c r="B16" s="6">
         <v>30</v>
@@ -1653,11 +1365,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H16" s="7">
@@ -1669,32 +1381,18 @@
         <v>70</v>
       </c>
       <c r="J16" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W16" s="15">
-        <v>10</v>
-      </c>
-      <c r="X16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y16" s="16">
-        <v>2</v>
-      </c>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27">
-        <f t="shared" si="3"/>
-        <v>44011</v>
+        <v>43997</v>
       </c>
       <c r="B17" s="6">
         <v>30</v>
@@ -1703,11 +1401,11 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H17" s="7">
@@ -1719,32 +1417,18 @@
         <v>70</v>
       </c>
       <c r="J17" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W17" s="15">
-        <v>11</v>
-      </c>
-      <c r="X17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y17" s="16">
-        <v>3</v>
-      </c>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <f t="shared" si="3"/>
-        <v>44025</v>
+        <v>44011</v>
       </c>
       <c r="B18" s="6">
         <v>30</v>
@@ -1753,11 +1437,11 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H18" s="7">
@@ -1769,29 +1453,18 @@
         <v>70</v>
       </c>
       <c r="J18" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K18" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W18" s="15">
-        <v>12</v>
-      </c>
-      <c r="X18" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y18" s="16">
-        <v>8</v>
-      </c>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-    </row>
-    <row r="19" spans="1:28" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <f t="shared" si="3"/>
-        <v>44039</v>
+        <v>44025</v>
       </c>
       <c r="B19" s="6">
         <v>30</v>
@@ -1800,11 +1473,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H19" s="7">
@@ -1816,29 +1489,18 @@
         <v>70</v>
       </c>
       <c r="J19" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W19" s="15">
-        <v>13</v>
-      </c>
-      <c r="X19" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y19" s="16">
-        <v>8</v>
-      </c>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-    </row>
-    <row r="20" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27">
-        <f t="shared" si="3"/>
-        <v>44053</v>
+        <v>44039</v>
       </c>
       <c r="B20" s="6">
         <v>30</v>
@@ -1847,11 +1509,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H20" s="7">
@@ -1863,29 +1525,18 @@
         <v>70</v>
       </c>
       <c r="J20" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W20" s="15">
-        <v>14</v>
-      </c>
-      <c r="X20" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y20" s="16">
-        <v>8</v>
-      </c>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-    </row>
-    <row r="21" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27">
-        <f t="shared" si="3"/>
-        <v>44067</v>
+        <v>44053</v>
       </c>
       <c r="B21" s="6">
         <v>30</v>
@@ -1894,11 +1545,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H21" s="7">
@@ -1910,31 +1561,18 @@
         <v>70</v>
       </c>
       <c r="J21" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W21" s="18">
-        <v>15</v>
-      </c>
-      <c r="X21" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y21" s="20">
-        <v>5</v>
-      </c>
-      <c r="Z21" s="19"/>
-      <c r="AA21" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <f t="shared" si="3"/>
-        <v>44081</v>
+        <v>44067</v>
       </c>
       <c r="B22" s="6">
         <v>30</v>
@@ -1943,11 +1581,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H22" s="7">
@@ -1959,28 +1597,18 @@
         <v>70</v>
       </c>
       <c r="J22" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K22" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-      <c r="W22" s="21">
-        <v>16</v>
-      </c>
-      <c r="X22" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y22" s="23">
-        <v>2</v>
-      </c>
-      <c r="Z22" s="24"/>
-    </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
-        <f t="shared" si="3"/>
-        <v>44095</v>
+        <v>44081</v>
       </c>
       <c r="B23" s="6">
         <v>30</v>
@@ -1989,11 +1617,11 @@
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H23" s="7">
@@ -2005,18 +1633,18 @@
         <v>70</v>
       </c>
       <c r="J23" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K23" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <f t="shared" si="3"/>
-        <v>44109</v>
+        <v>44095</v>
       </c>
       <c r="B24" s="6">
         <v>30</v>
@@ -2025,11 +1653,11 @@
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H24" s="7">
@@ -2041,18 +1669,18 @@
         <v>70</v>
       </c>
       <c r="J24" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K24" s="9">
+        <v>0.22857142857142856</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <f t="shared" si="2"/>
-        <v>0.22857142857142856</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <f t="shared" si="3"/>
-        <v>44123</v>
+        <v>44109</v>
       </c>
       <c r="B25" s="6">
         <v>30</v>
@@ -2061,11 +1689,11 @@
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="7">
-        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="H25" s="7">
@@ -2077,28 +1705,28 @@
         <v>70</v>
       </c>
       <c r="J25" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="9">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K25" s="9">
-        <f t="shared" si="2"/>
         <v>0.22857142857142856</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11">
         <f ca="1">SUM(B7:B31)</f>
-        <v>0</v>
+        <v>230</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11">
         <f ca="1">AVERAGE(D7:D52)</f>
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E26" s="11">
         <f ca="1">AVERAGE(E7:E52)</f>
-        <v>20.833333333333332</v>
+        <v>19.166666666666668</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -2113,8 +1741,7 @@
     <mergeCell ref="A5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>